<commit_message>
added html for excel file
</commit_message>
<xml_diff>
--- a/Results/Evaluation Measurements.xlsx
+++ b/Results/Evaluation Measurements.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfeif\Google Drive\01 Universität\6. Semester (SS 2017)\Verteilte Systeme\2018\PS\Project\Time Measurements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E093759A-D294-4CBF-A87F-F09F5127F2C0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{BFB40A1B-4F1C-4E42-8B49-8DCC72E3B8DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="Measurement Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>Instance-Type</t>
   </si>
@@ -113,17 +107,20 @@
   <si>
     <t>Up to 10 GBit/s</t>
   </si>
+  <si>
+    <t>Measured [MB/s]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
-    <numFmt numFmtId="170" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -518,34 +515,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -579,11 +548,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,68 +582,96 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,18 +691,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -720,7 +720,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -728,36 +728,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -768,7 +744,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -779,7 +754,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -794,7 +768,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -808,11 +781,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -823,7 +793,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -831,8 +801,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -843,7 +811,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -851,8 +819,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -863,7 +829,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -871,8 +837,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -883,7 +847,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -891,8 +855,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -903,7 +865,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -986,7 +948,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1869-46A9-939D-00AF5B36A68D}"/>
             </c:ext>
@@ -1005,11 +967,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1020,7 +979,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1028,8 +987,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1040,7 +997,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1048,8 +1005,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1060,7 +1015,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1068,8 +1023,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1080,7 +1033,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1088,8 +1041,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1100,7 +1051,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1108,8 +1059,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -1120,7 +1069,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000E-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1128,8 +1077,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -1140,7 +1087,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-1869-46A9-939D-00AF5B36A68D}"/>
               </c:ext>
@@ -1223,36 +1170,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1869-46A9-939D-00AF5B36A68D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="box"/>
-        <c:axId val="366156504"/>
-        <c:axId val="366158144"/>
+        <c:axId val="51894528"/>
+        <c:axId val="51773440"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="366156504"/>
+        <c:axId val="51894528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1281,23 +1218,20 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366158144"/>
+        <c:crossAx val="51773440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="366158144"/>
+        <c:axId val="51773440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1326,7 +1260,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366156504"/>
+        <c:crossAx val="51894528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1340,14 +1274,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1376,25 +1309,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1422,7 +1345,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1430,36 +1353,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1470,7 +1369,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1481,7 +1379,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1496,7 +1393,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1510,11 +1406,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1525,7 +1418,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1533,8 +1426,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1545,7 +1436,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1553,8 +1444,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1565,7 +1454,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1573,8 +1462,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1585,7 +1472,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1593,8 +1480,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1605,7 +1490,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1688,7 +1573,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C288-4EF0-9E9A-7670FD843F0B}"/>
             </c:ext>
@@ -1707,11 +1592,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1722,7 +1604,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1730,8 +1612,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1742,7 +1622,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1750,8 +1630,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1762,7 +1640,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1770,8 +1648,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1782,7 +1658,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1790,8 +1666,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1802,7 +1676,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1810,8 +1684,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -1822,7 +1694,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1830,8 +1702,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -1842,7 +1712,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-C288-4EF0-9E9A-7670FD843F0B}"/>
               </c:ext>
@@ -1925,36 +1795,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C288-4EF0-9E9A-7670FD843F0B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="box"/>
-        <c:axId val="464573944"/>
-        <c:axId val="464569024"/>
+        <c:axId val="51834880"/>
+        <c:axId val="51836416"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="464573944"/>
+        <c:axId val="51834880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1983,19 +1843,17 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464569024"/>
+        <c:crossAx val="51836416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="464569024"/>
+        <c:axId val="51836416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2013,7 +1871,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2042,7 +1899,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="464573944"/>
+        <c:crossAx val="51834880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2056,14 +1913,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2092,25 +1948,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2139,7 +1985,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2147,36 +1993,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2187,7 +2009,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2198,7 +2019,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2213,7 +2033,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2227,11 +2046,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2242,7 +2058,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2250,8 +2066,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2262,7 +2076,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2270,8 +2084,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2282,7 +2094,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2290,8 +2102,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2302,7 +2112,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2310,8 +2120,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2322,7 +2130,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2330,7 +2138,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Measurement Results'!$O$5:$O$14</c:f>
+              <c:f>'Measurement Results'!$P$5:$P$14</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2368,7 +2176,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Measurement Results'!$P$5:$P$14</c:f>
+              <c:f>'Measurement Results'!$Q$5:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* "-"????_ ;_-@_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -2405,7 +2213,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-899B-4CFA-A7A5-6F823BC26244}"/>
             </c:ext>
@@ -2424,11 +2232,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2439,7 +2244,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2447,8 +2252,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2459,7 +2262,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2467,8 +2270,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2479,7 +2280,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2487,8 +2288,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2499,7 +2298,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2507,8 +2306,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2519,7 +2316,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2527,8 +2324,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -2539,7 +2334,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000E-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2547,8 +2342,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -2559,7 +2352,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-899B-4CFA-A7A5-6F823BC26244}"/>
               </c:ext>
@@ -2567,7 +2360,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Measurement Results'!$O$5:$O$14</c:f>
+              <c:f>'Measurement Results'!$P$5:$P$14</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2605,7 +2398,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Measurement Results'!$R$5:$R$14</c:f>
+              <c:f>'Measurement Results'!$S$5:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* "-"????_ ;_-@_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -2642,36 +2435,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-899B-4CFA-A7A5-6F823BC26244}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="box"/>
-        <c:axId val="371684832"/>
-        <c:axId val="371685160"/>
+        <c:axId val="52110848"/>
+        <c:axId val="52112384"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="371684832"/>
+        <c:axId val="52110848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2700,19 +2483,17 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371685160"/>
+        <c:crossAx val="52112384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="371685160"/>
+        <c:axId val="52112384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2730,7 +2511,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="_-[$$-409]* #,##0.000_ ;_-[$$-409]* \-#,##0.000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2759,7 +2539,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371684832"/>
+        <c:crossAx val="52110848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2773,14 +2553,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2809,25 +2588,15 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-AT"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2855,7 +2624,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2863,36 +2632,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2903,7 +2648,6 @@
       </c:spPr>
     </c:floor>
     <c:sideWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2914,7 +2658,6 @@
       </c:spPr>
     </c:sideWall>
     <c:backWall>
-      <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2929,7 +2672,6 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2943,11 +2685,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2958,7 +2697,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -2966,8 +2705,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2978,7 +2715,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -2986,8 +2723,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -2998,7 +2733,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3006,8 +2741,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3018,7 +2751,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3026,8 +2759,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3038,7 +2769,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3046,7 +2777,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Measurement Results'!$O$5:$O$14</c:f>
+              <c:f>'Measurement Results'!$P$5:$P$14</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -3084,7 +2815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Measurement Results'!$Q$5:$Q$14</c:f>
+              <c:f>'Measurement Results'!$R$5:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"????_ ;_-@_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -3121,7 +2852,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9094-47AD-8D01-65C8F88BA962}"/>
             </c:ext>
@@ -3140,11 +2871,8 @@
             <a:effectLst/>
             <a:sp3d/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3155,7 +2883,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3163,8 +2891,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3175,7 +2901,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3183,8 +2909,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3195,7 +2919,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3203,8 +2927,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3215,7 +2937,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3223,8 +2945,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -3235,7 +2955,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3243,8 +2963,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -3255,7 +2973,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3263,8 +2981,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -3275,7 +2991,7 @@
               <a:effectLst/>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-9094-47AD-8D01-65C8F88BA962}"/>
               </c:ext>
@@ -3283,7 +2999,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Measurement Results'!$O$5:$O$14</c:f>
+              <c:f>'Measurement Results'!$P$5:$P$14</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -3321,7 +3037,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Measurement Results'!$S$5:$S$14</c:f>
+              <c:f>'Measurement Results'!$T$5:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* "-"????_ ;_-@_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -3358,36 +3074,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9094-47AD-8D01-65C8F88BA962}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="box"/>
-        <c:axId val="474382096"/>
-        <c:axId val="474394888"/>
+        <c:axId val="53226496"/>
+        <c:axId val="53244672"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="474382096"/>
+        <c:axId val="53226496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3416,19 +3122,17 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474394888"/>
+        <c:crossAx val="53244672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474394888"/>
+        <c:axId val="53244672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3446,7 +3150,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ " sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3475,7 +3178,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474382096"/>
+        <c:crossAx val="53226496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3489,14 +3192,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3525,7 +3227,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5687,7 +5389,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05549AA5-2D39-42FD-8606-6A757FFDBDF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{05549AA5-2D39-42FD-8606-6A757FFDBDF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5723,7 +5425,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87668F05-33BD-4E60-AE3A-E10A6A72DE84}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{87668F05-33BD-4E60-AE3A-E10A6A72DE84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5759,7 +5461,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10448BB5-C9F0-430D-883C-889A761F5CF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{10448BB5-C9F0-430D-883C-889A761F5CF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5795,7 +5497,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{476B63CA-7C14-414B-AF69-60CAC643DC0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{476B63CA-7C14-414B-AF69-60CAC643DC0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5859,7 +5561,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5911,7 +5613,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6105,21 +5807,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48ABFD93-B854-4EB6-9561-29DAC20DC0B4}">
-  <dimension ref="B3:S37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
@@ -6133,16 +5835,17 @@
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
     <col min="17" max="17" width="15.28515625" customWidth="1"/>
     <col min="18" max="18" width="15.85546875" customWidth="1"/>
     <col min="19" max="19" width="15.5703125" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="15.75" thickBot="1"/>
+    <row r="4" spans="2:20" ht="15.75" thickBot="1">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -6168,29 +5871,32 @@
       <c r="J4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="42" t="s">
+      <c r="N4" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="Q4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="43" t="s">
+      <c r="R4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="S4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="44" t="s">
+      <c r="T4" s="31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -6200,7 +5906,7 @@
       <c r="D5" s="7">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -6212,526 +5918,552 @@
       <c r="I5" s="7">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="L5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="M5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="N5" s="33">
+        <v>24.047699999999999</v>
+      </c>
+      <c r="P5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="23">
+      <c r="Q5" s="15">
         <f>(D5 / (C5*3600) ) * 1000000</f>
         <v>4.0428906806980386E-2</v>
       </c>
-      <c r="Q5" s="24">
-        <f xml:space="preserve"> P5 ^(-1)</f>
+      <c r="R5" s="16">
+        <f xml:space="preserve"> Q5 ^(-1)</f>
         <v>24.734777142857144</v>
       </c>
-      <c r="R5" s="25">
+      <c r="S5" s="17">
         <f>(I5 / (H5*3600) ) * 1000000</f>
         <v>4.398326060437293E-2</v>
       </c>
-      <c r="S5" s="26">
-        <f xml:space="preserve"> R5 ^(-1)</f>
+      <c r="T5" s="18">
+        <f xml:space="preserve"> S5 ^(-1)</f>
         <v>22.7359224</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:20">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>36.703474999999997</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>36.100050000000003</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="46" t="s">
+      <c r="M6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="N6" s="34">
+        <v>36.703474999999997</v>
+      </c>
+      <c r="P6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="28">
+      <c r="Q6" s="20">
         <f>(D6 / (C6*3600) ) * 1000000</f>
         <v>5.2220305207249913E-2</v>
       </c>
-      <c r="Q6" s="29">
-        <f t="shared" ref="Q6:Q14" si="0" xml:space="preserve"> P6 ^(-1)</f>
+      <c r="R6" s="21">
+        <f t="shared" ref="R6:R14" si="0" xml:space="preserve"> Q6 ^(-1)</f>
         <v>19.149639130434778</v>
       </c>
-      <c r="R6" s="30">
+      <c r="S6" s="22">
         <f>(I6 / (H6*3600) ) * 1000000</f>
         <v>5.3093185928181998E-2</v>
       </c>
-      <c r="S6" s="31">
-        <f t="shared" ref="S6:S14" si="1" xml:space="preserve"> R6 ^(-1)</f>
+      <c r="T6" s="23">
+        <f t="shared" ref="T6:T14" si="1" xml:space="preserve"> S6 ^(-1)</f>
         <v>18.834808695652175</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:20">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>71.002931000000004</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>68.375956000000002</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="46" t="s">
+      <c r="M7" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="27" t="s">
+      <c r="N7" s="34">
+        <v>71.002931000000004</v>
+      </c>
+      <c r="P7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="28">
+      <c r="Q7" s="20">
         <f>(D7 / (C7*3600) ) * 1000000</f>
         <v>5.4379601753498187E-2</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="R7" s="21">
         <f t="shared" si="0"/>
         <v>18.389248316546762</v>
       </c>
-      <c r="R7" s="30">
+      <c r="S7" s="22">
         <f>(I7 / (H7*3600) ) * 1000000</f>
         <v>5.6468842806543143E-2</v>
       </c>
-      <c r="S7" s="31">
+      <c r="T7" s="23">
         <f t="shared" si="1"/>
         <v>17.708880690647486</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:20">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>93.105728999999997</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>2.7799999999999998E-2</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>89.669032000000001</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>2.7799999999999998E-2</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="N8" s="34">
+        <v>93.105728999999997</v>
+      </c>
+      <c r="P8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="28">
+      <c r="Q8" s="20">
         <f>(D8 / (C8*3600) ) * 1000000</f>
         <v>8.2940355069044389E-2</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="R8" s="21">
         <f t="shared" si="0"/>
         <v>12.056856992805754</v>
       </c>
-      <c r="R8" s="30">
+      <c r="S8" s="22">
         <f>(I8 / (H8*3600) ) * 1000000</f>
         <v>8.6119165669394329E-2</v>
       </c>
-      <c r="S8" s="31">
+      <c r="T8" s="23">
         <f t="shared" si="1"/>
         <v>11.611817093525181</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:20">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>112.72880000000001</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>5.57E-2</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>119.178847</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>5.57E-2</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="N9" s="34">
+        <v>112.72880000000001</v>
+      </c>
+      <c r="P9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="28">
+      <c r="Q9" s="20">
         <f>(D9 / (C9*3600) ) * 1000000</f>
         <v>0.13725172468989486</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="R9" s="21">
         <f t="shared" si="0"/>
         <v>7.2858829443447055</v>
       </c>
-      <c r="R9" s="30">
+      <c r="S9" s="22">
         <f>(I9 / (H9*3600) ) * 1000000</f>
         <v>0.12982356023483113</v>
       </c>
-      <c r="S9" s="31">
+      <c r="T9" s="23">
         <f t="shared" si="1"/>
         <v>7.7027621041292633</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:20">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>133.36751000000001</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>1.6299999999999999E-2</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>136.253007</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>2.5100000000000001E-2</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="27" t="s">
+      <c r="N10" s="34">
+        <v>133.36751000000001</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="28">
+      <c r="Q10" s="20">
         <f>(D10 / (C10*3600) ) * 1000000</f>
         <v>3.3949631194117501E-2</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="R10" s="21">
         <f t="shared" si="0"/>
         <v>29.455400981595091</v>
       </c>
-      <c r="R10" s="30">
+      <c r="S10" s="22">
         <f>(I10 / (H10*3600) ) * 1000000</f>
         <v>5.1171143857560684E-2</v>
       </c>
-      <c r="S10" s="31">
+      <c r="T10" s="23">
         <f t="shared" si="1"/>
         <v>19.542263952191234</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="2:20">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>178.24399500000001</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>3.2599999999999997E-2</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>182.129052</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>5.0299999999999997E-2</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="47" t="s">
+      <c r="M11" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="27" t="s">
+      <c r="N11" s="34">
+        <v>178.24399500000001</v>
+      </c>
+      <c r="P11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="28">
+      <c r="Q11" s="20">
         <f>(D11 / (C11*3600) ) * 1000000</f>
         <v>5.0804267238038249E-2</v>
       </c>
-      <c r="Q11" s="29">
+      <c r="R11" s="21">
         <f t="shared" si="0"/>
         <v>19.68338595092025</v>
       </c>
-      <c r="R11" s="30">
+      <c r="S11" s="22">
         <f>(I11 / (H11*3600) ) * 1000000</f>
         <v>7.6716054186798388E-2</v>
       </c>
-      <c r="S11" s="31">
+      <c r="T11" s="23">
         <f t="shared" si="1"/>
         <v>13.035081256461233</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="2:20">
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>206.25083100000001</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>7.1099999999999997E-2</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>202.745813</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>0.10059999999999999</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="N12" s="34">
+        <v>206.25083100000001</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="28">
+      <c r="Q12" s="20">
         <f>(D12 / (C12*3600) ) * 1000000</f>
         <v>9.5757189943152257E-2</v>
       </c>
-      <c r="Q12" s="29">
+      <c r="R12" s="21">
         <f t="shared" si="0"/>
         <v>10.443080050632913</v>
       </c>
-      <c r="R12" s="30">
+      <c r="S12" s="22">
         <f>(I12 / (H12*3600) ) * 1000000</f>
         <v>0.13782994593552686</v>
       </c>
-      <c r="S12" s="31">
+      <c r="T12" s="23">
         <f t="shared" si="1"/>
         <v>7.2553173638170989</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:20">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>136.495497</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>1.6799999999999999E-2</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>131.58600799999999</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="27" t="s">
+      <c r="N13" s="34">
+        <v>136.495497</v>
+      </c>
+      <c r="P13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="28">
+      <c r="Q13" s="20">
         <f>(D13 / (C13*3600) ) * 1000000</f>
         <v>3.4189162054676911E-2</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="R13" s="21">
         <f t="shared" si="0"/>
         <v>29.249035071428576</v>
       </c>
-      <c r="R13" s="30">
+      <c r="S13" s="22">
         <f>(I13 / (H13*3600) ) * 1000000</f>
         <v>4.6230852548800883E-2</v>
       </c>
-      <c r="S13" s="31">
+      <c r="T13" s="23">
         <f t="shared" si="1"/>
         <v>21.630576657534245</v>
       </c>
     </row>
-    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+    <row r="14" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>176.79127800000001</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="13">
         <v>3.61E-2</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="12">
         <v>184.98437799999999</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="13">
         <v>4.3700000000000003E-2</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="48" t="s">
+      <c r="M14" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="N14" s="35">
+        <v>176.79127800000001</v>
+      </c>
+      <c r="P14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="P14" s="33">
+      <c r="Q14" s="25">
         <f>(D14 / (C14*3600) ) * 1000000</f>
         <v>5.6720998293692849E-2</v>
       </c>
-      <c r="Q14" s="34">
+      <c r="R14" s="26">
         <f t="shared" si="0"/>
         <v>17.630155146814403</v>
       </c>
-      <c r="R14" s="35">
+      <c r="S14" s="27">
         <f>(I14 / (H14*3600) ) * 1000000</f>
         <v>6.5621156878927847E-2</v>
       </c>
-      <c r="S14" s="36">
+      <c r="T14" s="28">
         <f t="shared" si="1"/>
         <v>15.238987661327231</v>
       </c>
     </row>
-    <row r="32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="11:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K33" s="37" t="s">
+    <row r="33" spans="11:11">
+      <c r="K33" s="48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34" s="38" t="s">
+    <row r="34" spans="11:11">
+      <c r="K34" s="49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="39" t="s">
+    <row r="35" spans="11:11">
+      <c r="K35" s="50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="40" t="s">
+    <row r="36" spans="11:11">
+      <c r="K36" s="51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="11:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K37" s="41" t="s">
+    <row r="37" spans="11:11">
+      <c r="K37" s="52" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="R5:R14" formula="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>